<commit_message>
some updates to the sample Excel file
</commit_message>
<xml_diff>
--- a/miscs/day-4_sample.xlsx
+++ b/miscs/day-4_sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/Data/haradatm/kenkyu/250621/gssm/03-samples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/Data/haradatm/kenkyu/250726/gssm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD5936A-12E0-4043-A6B9-93D47BF05018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39DDB0C-4AEE-B744-A7B6-88326556E081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9220" yWindow="3600" windowWidth="27900" windowHeight="16840" xr2:uid="{B77AEB33-BBB0-A24C-90E1-B4FC197890F3}"/>
+    <workbookView xWindow="6300" yWindow="3600" windowWidth="27900" windowHeight="16840" xr2:uid="{B77AEB33-BBB0-A24C-90E1-B4FC197890F3}"/>
   </bookViews>
   <sheets>
     <sheet name="特徴語の集計" sheetId="1" r:id="rId1"/>
@@ -245,7 +245,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode=".000"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -312,22 +312,6 @@
     <font>
       <sz val="11"/>
       <color theme="7" tint="-0.249977111117893"/>
-      <name val="Meiryo UI"/>
-      <family val="2"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color rgb="FF7030A0"/>
-      <name val="Meiryo UI"/>
-      <family val="2"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Meiryo UI"/>
       <family val="2"/>
       <charset val="128"/>
@@ -481,9 +465,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -493,13 +474,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -510,7 +488,7 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -522,11 +500,17 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -847,25 +831,25 @@
   <dimension ref="A2:U28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.5703125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="2" width="7.5703125" style="19"/>
-    <col min="3" max="3" width="1.42578125" style="20" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.28515625" style="20" customWidth="1"/>
-    <col min="6" max="7" width="7.5703125" style="19"/>
-    <col min="8" max="8" width="1.42578125" style="19" customWidth="1"/>
-    <col min="9" max="10" width="7.5703125" style="19"/>
-    <col min="11" max="11" width="1.42578125" style="19" customWidth="1"/>
-    <col min="12" max="13" width="7.5703125" style="19"/>
-    <col min="14" max="14" width="1.42578125" style="19" customWidth="1"/>
-    <col min="15" max="16" width="7.5703125" style="19"/>
-    <col min="17" max="17" width="1.42578125" style="19" customWidth="1"/>
-    <col min="18" max="21" width="7.5703125" style="19"/>
-    <col min="22" max="16384" width="7.5703125" style="20"/>
+    <col min="1" max="2" width="7.5703125" style="17"/>
+    <col min="3" max="3" width="1.42578125" style="18" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.28515625" style="18" customWidth="1"/>
+    <col min="6" max="7" width="7.5703125" style="17"/>
+    <col min="8" max="8" width="1.42578125" style="17" customWidth="1"/>
+    <col min="9" max="10" width="7.5703125" style="17"/>
+    <col min="11" max="11" width="1.42578125" style="17" customWidth="1"/>
+    <col min="12" max="13" width="7.5703125" style="17"/>
+    <col min="14" max="14" width="1.42578125" style="17" customWidth="1"/>
+    <col min="15" max="16" width="7.5703125" style="17"/>
+    <col min="17" max="17" width="1.42578125" style="17" customWidth="1"/>
+    <col min="18" max="21" width="7.5703125" style="17"/>
+    <col min="22" max="16384" width="7.5703125" style="18"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
@@ -904,7 +888,7 @@
       <c r="U2" s="4"/>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="6">
@@ -913,35 +897,35 @@
       <c r="D3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="19" t="s">
         <v>24</v>
       </c>
       <c r="G3" s="6">
         <v>0.125175808720112</v>
       </c>
       <c r="H3" s="4"/>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="19" t="s">
         <v>24</v>
       </c>
       <c r="J3" s="6">
         <v>0.13582584003786</v>
       </c>
       <c r="K3" s="4"/>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="19" t="s">
         <v>20</v>
       </c>
       <c r="M3" s="6">
         <v>0.13709160794362499</v>
       </c>
       <c r="N3" s="4"/>
-      <c r="O3" s="5" t="s">
+      <c r="O3" s="19" t="s">
         <v>24</v>
       </c>
       <c r="P3" s="6">
         <v>0.11992533831077901</v>
       </c>
       <c r="Q3" s="4"/>
-      <c r="R3" s="5" t="s">
+      <c r="R3" s="20" t="s">
         <v>22</v>
       </c>
       <c r="S3" s="6">
@@ -960,35 +944,35 @@
       <c r="D4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="19" t="s">
         <v>25</v>
       </c>
       <c r="G4" s="6">
         <v>0.105948609644491</v>
       </c>
       <c r="H4" s="4"/>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="19" t="s">
         <v>25</v>
       </c>
       <c r="J4" s="6">
         <v>0.130215827338129</v>
       </c>
       <c r="K4" s="4"/>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="23" t="s">
         <v>33</v>
       </c>
       <c r="M4" s="6">
         <v>0.13136227544910101</v>
       </c>
       <c r="N4" s="4"/>
-      <c r="O4" s="5" t="s">
+      <c r="O4" s="24" t="s">
         <v>8</v>
       </c>
       <c r="P4" s="6">
         <v>7.8473722102231802E-2</v>
       </c>
       <c r="Q4" s="4"/>
-      <c r="R4" s="5" t="s">
+      <c r="R4" s="23" t="s">
         <v>33</v>
       </c>
       <c r="S4" s="6">
@@ -998,7 +982,7 @@
       <c r="U4" s="4"/>
     </row>
     <row r="5" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="23" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="6">
@@ -1007,14 +991,14 @@
       <c r="D5" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="23" t="s">
         <v>33</v>
       </c>
       <c r="G5" s="6">
         <v>9.7676107480029001E-2</v>
       </c>
       <c r="H5" s="4"/>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="24" t="s">
         <v>22</v>
       </c>
       <c r="J5" s="6">
@@ -1028,14 +1012,14 @@
         <v>0.10580766517752099</v>
       </c>
       <c r="N5" s="4"/>
-      <c r="O5" s="5" t="s">
+      <c r="O5" s="21" t="s">
         <v>3</v>
       </c>
       <c r="P5" s="6">
         <v>7.3542600896860905E-2</v>
       </c>
       <c r="Q5" s="4"/>
-      <c r="R5" s="5" t="s">
+      <c r="R5" s="19" t="s">
         <v>20</v>
       </c>
       <c r="S5" s="6">
@@ -1045,7 +1029,7 @@
       <c r="U5" s="4"/>
     </row>
     <row r="6" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="19" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="6">
@@ -1061,14 +1045,14 @@
         <v>9.2450638792102205E-2</v>
       </c>
       <c r="H6" s="4"/>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="23" t="s">
         <v>33</v>
       </c>
       <c r="J6" s="6">
         <v>0.105705925384052</v>
       </c>
       <c r="K6" s="4"/>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="20" t="s">
         <v>7</v>
       </c>
       <c r="M6" s="6">
@@ -1082,7 +1066,7 @@
         <v>6.6115702479338803E-2</v>
       </c>
       <c r="Q6" s="4"/>
-      <c r="R6" s="5" t="s">
+      <c r="R6" s="19" t="s">
         <v>24</v>
       </c>
       <c r="S6" s="6">
@@ -1092,7 +1076,7 @@
       <c r="U6" s="4"/>
     </row>
     <row r="7" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="19" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="6">
@@ -1101,7 +1085,7 @@
       <c r="D7" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="23" t="s">
         <v>18</v>
       </c>
       <c r="G7" s="6">
@@ -1115,21 +1099,21 @@
         <v>0.103472548099483</v>
       </c>
       <c r="K7" s="4"/>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="19" t="s">
         <v>24</v>
       </c>
       <c r="M7" s="6">
         <v>0.10091743119266</v>
       </c>
       <c r="N7" s="4"/>
-      <c r="O7" s="5" t="s">
+      <c r="O7" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P7" s="6">
         <v>6.1383928571428499E-2</v>
       </c>
       <c r="Q7" s="4"/>
-      <c r="R7" s="5" t="s">
+      <c r="R7" s="19" t="s">
         <v>25</v>
       </c>
       <c r="S7" s="6">
@@ -1139,13 +1123,13 @@
       <c r="U7" s="4"/>
     </row>
     <row r="8" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="22" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="6">
         <v>0.15521305530371701</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="16" t="s">
         <v>23</v>
       </c>
       <c r="F8" s="5" t="s">
@@ -1155,28 +1139,28 @@
         <v>8.0440771349862203E-2</v>
       </c>
       <c r="H8" s="4"/>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="20" t="s">
         <v>7</v>
       </c>
       <c r="J8" s="6">
         <v>9.7983295986962704E-2</v>
       </c>
       <c r="K8" s="4"/>
-      <c r="L8" s="5" t="s">
+      <c r="L8" s="19" t="s">
         <v>25</v>
       </c>
       <c r="M8" s="6">
         <v>0.100525394045534</v>
       </c>
       <c r="N8" s="4"/>
-      <c r="O8" s="5" t="s">
+      <c r="O8" s="24" t="s">
         <v>49</v>
       </c>
       <c r="P8" s="6">
         <v>5.7115198451113201E-2</v>
       </c>
       <c r="Q8" s="4"/>
-      <c r="R8" s="5" t="s">
+      <c r="R8" s="22" t="s">
         <v>21</v>
       </c>
       <c r="S8" s="6">
@@ -1186,34 +1170,34 @@
       <c r="U8" s="4"/>
     </row>
     <row r="9" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="24" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="6">
         <v>0.147731755424063</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="23" t="s">
         <v>43</v>
       </c>
       <c r="G9" s="6">
         <v>8.0086580086579998E-2</v>
       </c>
       <c r="H9" s="4"/>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="22" t="s">
         <v>21</v>
       </c>
       <c r="J9" s="6">
         <v>8.8613406795224905E-2</v>
       </c>
       <c r="K9" s="4"/>
-      <c r="L9" s="5" t="s">
+      <c r="L9" s="23" t="s">
         <v>18</v>
       </c>
       <c r="M9" s="6">
         <v>9.7240473061760799E-2</v>
       </c>
       <c r="N9" s="4"/>
-      <c r="O9" s="5" t="s">
+      <c r="O9" s="21" t="s">
         <v>35</v>
       </c>
       <c r="P9" s="6">
@@ -1230,7 +1214,7 @@
       <c r="U9" s="4"/>
     </row>
     <row r="10" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="19" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="6">
@@ -1243,28 +1227,28 @@
         <v>7.4556213017751394E-2</v>
       </c>
       <c r="H10" s="4"/>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="19" t="s">
         <v>48</v>
       </c>
       <c r="J10" s="6">
         <v>8.6038961038960998E-2</v>
       </c>
       <c r="K10" s="4"/>
-      <c r="L10" s="5" t="s">
+      <c r="L10" s="20" t="s">
         <v>22</v>
       </c>
       <c r="M10" s="6">
         <v>9.11817636472705E-2</v>
       </c>
       <c r="N10" s="4"/>
-      <c r="O10" s="5" t="s">
+      <c r="O10" s="22" t="s">
         <v>2</v>
       </c>
       <c r="P10" s="6">
         <v>5.3691275167785199E-2</v>
       </c>
       <c r="Q10" s="4"/>
-      <c r="R10" s="5" t="s">
+      <c r="R10" s="20" t="s">
         <v>7</v>
       </c>
       <c r="S10" s="6">
@@ -1280,7 +1264,7 @@
       <c r="B11" s="6">
         <v>0.131295981890209</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="19" t="s">
         <v>20</v>
       </c>
       <c r="G11" s="6">
@@ -1294,7 +1278,7 @@
         <v>8.4147665580890305E-2</v>
       </c>
       <c r="K11" s="4"/>
-      <c r="L11" s="5" t="s">
+      <c r="L11" s="22" t="s">
         <v>21</v>
       </c>
       <c r="M11" s="6">
@@ -1308,7 +1292,7 @@
         <v>5.2183173588924298E-2</v>
       </c>
       <c r="Q11" s="4"/>
-      <c r="R11" s="5" t="s">
+      <c r="R11" s="23" t="s">
         <v>18</v>
       </c>
       <c r="S11" s="6">
@@ -1318,44 +1302,44 @@
       <c r="U11" s="4"/>
     </row>
     <row r="12" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="13">
         <v>0.12254999010096999</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="13">
         <v>7.0777479892761397E-2</v>
       </c>
-      <c r="H12" s="15"/>
-      <c r="I12" s="13" t="s">
+      <c r="H12" s="14"/>
+      <c r="I12" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="J12" s="14">
+      <c r="J12" s="13">
         <v>8.0908445706174503E-2</v>
       </c>
-      <c r="K12" s="15"/>
-      <c r="L12" s="13" t="s">
+      <c r="K12" s="14"/>
+      <c r="L12" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="M12" s="14">
+      <c r="M12" s="13">
         <v>8.5714285714285701E-2</v>
       </c>
-      <c r="N12" s="15"/>
-      <c r="O12" s="13" t="s">
+      <c r="N12" s="14"/>
+      <c r="O12" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="P12" s="14">
+      <c r="P12" s="13">
         <v>4.7445255474452497E-2</v>
       </c>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="13" t="s">
+      <c r="Q12" s="14"/>
+      <c r="R12" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="S12" s="14">
+      <c r="S12" s="13">
         <v>9.4833687190374993E-2</v>
       </c>
       <c r="T12" s="4"/>
@@ -1417,44 +1401,44 @@
       <c r="U14" s="4"/>
     </row>
     <row r="15" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="24" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="6">
         <v>0.21606118546845099</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="24" t="s">
         <v>8</v>
       </c>
       <c r="G15" s="6">
         <v>9.6231247713135695E-2</v>
       </c>
       <c r="H15" s="4"/>
-      <c r="I15" s="5" t="s">
+      <c r="I15" s="24" t="s">
         <v>8</v>
       </c>
       <c r="J15" s="6">
         <v>8.8267344714856505E-2</v>
       </c>
       <c r="K15" s="4"/>
-      <c r="L15" s="5" t="s">
+      <c r="L15" s="21" t="s">
         <v>1</v>
       </c>
       <c r="M15" s="6">
         <v>0.122837370242214</v>
       </c>
       <c r="N15" s="4"/>
-      <c r="O15" s="5" t="s">
+      <c r="O15" s="21" t="s">
         <v>1</v>
       </c>
       <c r="P15" s="6">
         <v>9.9378881987577605E-2</v>
       </c>
       <c r="Q15" s="4"/>
-      <c r="R15" s="5" t="s">
+      <c r="R15" s="24" t="s">
         <v>8</v>
       </c>
       <c r="S15" s="6">
@@ -1464,7 +1448,7 @@
       <c r="U15" s="4"/>
     </row>
     <row r="16" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="21" t="s">
         <v>1</v>
       </c>
       <c r="B16" s="6">
@@ -1473,35 +1457,35 @@
       <c r="D16" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="21" t="s">
         <v>35</v>
       </c>
       <c r="G16" s="6">
         <v>8.3068783068783E-2</v>
       </c>
       <c r="H16" s="4"/>
-      <c r="I16" s="5" t="s">
+      <c r="I16" s="21" t="s">
         <v>1</v>
       </c>
       <c r="J16" s="6">
         <v>7.0368334249587605E-2</v>
       </c>
       <c r="K16" s="4"/>
-      <c r="L16" s="5" t="s">
+      <c r="L16" s="21" t="s">
         <v>36</v>
       </c>
       <c r="M16" s="6">
         <v>8.29875518672199E-2</v>
       </c>
       <c r="N16" s="4"/>
-      <c r="O16" s="5" t="s">
+      <c r="O16" s="24" t="s">
         <v>8</v>
       </c>
       <c r="P16" s="6">
         <v>9.18367346938775E-2</v>
       </c>
       <c r="Q16" s="4"/>
-      <c r="R16" s="5" t="s">
+      <c r="R16" s="21" t="s">
         <v>3</v>
       </c>
       <c r="S16" s="6">
@@ -1511,44 +1495,44 @@
       <c r="U16" s="4"/>
     </row>
     <row r="17" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="21" t="s">
         <v>3</v>
       </c>
       <c r="B17" s="6">
         <v>0.15207207207207199</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="21" t="s">
         <v>3</v>
       </c>
       <c r="G17" s="6">
         <v>7.6438848920863306E-2</v>
       </c>
       <c r="H17" s="4"/>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="21" t="s">
         <v>35</v>
       </c>
       <c r="J17" s="6">
         <v>6.9487983281086699E-2</v>
       </c>
       <c r="K17" s="4"/>
-      <c r="L17" s="5" t="s">
+      <c r="L17" s="21" t="s">
         <v>35</v>
       </c>
       <c r="M17" s="6">
         <v>8.1923890063424903E-2</v>
       </c>
       <c r="N17" s="4"/>
-      <c r="O17" s="5" t="s">
+      <c r="O17" s="21" t="s">
         <v>35</v>
       </c>
       <c r="P17" s="6">
         <v>8.0211081794195199E-2</v>
       </c>
       <c r="Q17" s="4"/>
-      <c r="R17" s="5" t="s">
+      <c r="R17" s="21" t="s">
         <v>35</v>
       </c>
       <c r="S17" s="6">
@@ -1558,7 +1542,7 @@
       <c r="U17" s="4"/>
     </row>
     <row r="18" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="21" t="s">
         <v>35</v>
       </c>
       <c r="B18" s="6">
@@ -1567,35 +1551,35 @@
       <c r="D18" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="19" t="s">
         <v>40</v>
       </c>
       <c r="G18" s="6">
         <v>7.0343275182892503E-2</v>
       </c>
       <c r="H18" s="4"/>
-      <c r="I18" s="5" t="s">
+      <c r="I18" s="21" t="s">
         <v>3</v>
       </c>
       <c r="J18" s="6">
         <v>6.447309915518E-2</v>
       </c>
       <c r="K18" s="4"/>
-      <c r="L18" s="5" t="s">
+      <c r="L18" s="21" t="s">
         <v>45</v>
       </c>
       <c r="M18" s="6">
         <v>8.1323225361819407E-2</v>
       </c>
       <c r="N18" s="4"/>
-      <c r="O18" s="5" t="s">
+      <c r="O18" s="21" t="s">
         <v>3</v>
       </c>
       <c r="P18" s="6">
         <v>7.69230769230769E-2</v>
       </c>
       <c r="Q18" s="4"/>
-      <c r="R18" s="5" t="s">
+      <c r="R18" s="21" t="s">
         <v>1</v>
       </c>
       <c r="S18" s="6">
@@ -1605,7 +1589,7 @@
       <c r="U18" s="4"/>
     </row>
     <row r="19" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="21" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="6">
@@ -1614,14 +1598,14 @@
       <c r="D19" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="21" t="s">
         <v>1</v>
       </c>
       <c r="G19" s="6">
         <v>6.9780219780219699E-2</v>
       </c>
       <c r="H19" s="4"/>
-      <c r="I19" s="5" t="s">
+      <c r="I19" s="22" t="s">
         <v>2</v>
       </c>
       <c r="J19" s="6">
@@ -1635,14 +1619,14 @@
         <v>8.0808080808080801E-2</v>
       </c>
       <c r="N19" s="4"/>
-      <c r="O19" s="5" t="s">
+      <c r="O19" s="21" t="s">
         <v>36</v>
       </c>
       <c r="P19" s="6">
         <v>7.4705882352941094E-2</v>
       </c>
       <c r="Q19" s="4"/>
-      <c r="R19" s="5" t="s">
+      <c r="R19" s="21" t="s">
         <v>36</v>
       </c>
       <c r="S19" s="6">
@@ -1652,44 +1636,44 @@
       <c r="U19" s="4"/>
     </row>
     <row r="20" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="22" t="s">
         <v>2</v>
       </c>
       <c r="B20" s="6">
         <v>0.104561666979538</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="24" t="s">
         <v>39</v>
       </c>
       <c r="G20" s="6">
         <v>6.2573789846517097E-2</v>
       </c>
       <c r="H20" s="4"/>
-      <c r="I20" s="5" t="s">
+      <c r="I20" s="22" t="s">
         <v>44</v>
       </c>
       <c r="J20" s="6">
         <v>6.1292471685542901E-2</v>
       </c>
       <c r="K20" s="4"/>
-      <c r="L20" s="5" t="s">
+      <c r="L20" s="21" t="s">
         <v>3</v>
       </c>
       <c r="M20" s="6">
         <v>7.6438848920863306E-2</v>
       </c>
       <c r="N20" s="4"/>
-      <c r="O20" s="5" t="s">
+      <c r="O20" s="21" t="s">
         <v>45</v>
       </c>
       <c r="P20" s="6">
         <v>6.8801089918256106E-2</v>
       </c>
       <c r="Q20" s="4"/>
-      <c r="R20" s="5" t="s">
+      <c r="R20" s="22" t="s">
         <v>2</v>
       </c>
       <c r="S20" s="6">
@@ -1699,7 +1683,7 @@
       <c r="U20" s="4"/>
     </row>
     <row r="21" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="24" t="s">
         <v>56</v>
       </c>
       <c r="B21" s="6">
@@ -1712,28 +1696,28 @@
         <v>6.1577608142493599E-2</v>
       </c>
       <c r="H21" s="4"/>
-      <c r="I21" s="5" t="s">
+      <c r="I21" s="24" t="s">
         <v>38</v>
       </c>
       <c r="J21" s="6">
         <v>5.9421025901472802E-2</v>
       </c>
       <c r="K21" s="4"/>
-      <c r="L21" s="5" t="s">
+      <c r="L21" s="22" t="s">
         <v>2</v>
       </c>
       <c r="M21" s="6">
         <v>6.1408450704225299E-2</v>
       </c>
       <c r="N21" s="4"/>
-      <c r="O21" s="5" t="s">
+      <c r="O21" s="22" t="s">
         <v>2</v>
       </c>
       <c r="P21" s="6">
         <v>6.50084793668739E-2</v>
       </c>
       <c r="Q21" s="4"/>
-      <c r="R21" s="5" t="s">
+      <c r="R21" s="24" t="s">
         <v>39</v>
       </c>
       <c r="S21" s="6">
@@ -1743,7 +1727,7 @@
       <c r="U21" s="4"/>
     </row>
     <row r="22" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="24" t="s">
         <v>39</v>
       </c>
       <c r="B22" s="6">
@@ -1756,21 +1740,21 @@
         <v>5.9017941454202E-2</v>
       </c>
       <c r="H22" s="4"/>
-      <c r="I22" s="5" t="s">
+      <c r="I22" s="24" t="s">
         <v>39</v>
       </c>
       <c r="J22" s="6">
         <v>5.5099648300117203E-2</v>
       </c>
       <c r="K22" s="4"/>
-      <c r="L22" s="5" t="s">
+      <c r="L22" s="22" t="s">
         <v>44</v>
       </c>
       <c r="M22" s="6">
         <v>5.6366047745358E-2</v>
       </c>
       <c r="N22" s="4"/>
-      <c r="O22" s="5" t="s">
+      <c r="O22" s="24" t="s">
         <v>39</v>
       </c>
       <c r="P22" s="6">
@@ -1787,41 +1771,41 @@
       <c r="U22" s="4"/>
     </row>
     <row r="23" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="21" t="s">
         <v>45</v>
       </c>
       <c r="B23" s="6">
         <v>8.7270597422881693E-2</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="22" t="s">
         <v>2</v>
       </c>
       <c r="G23" s="6">
         <v>5.8426966292134799E-2</v>
       </c>
       <c r="H23" s="4"/>
-      <c r="I23" s="5" t="s">
+      <c r="I23" s="21" t="s">
         <v>36</v>
       </c>
       <c r="J23" s="6">
         <v>5.4849884526558798E-2</v>
       </c>
       <c r="K23" s="4"/>
-      <c r="L23" s="5" t="s">
+      <c r="L23" s="24" t="s">
         <v>39</v>
       </c>
       <c r="M23" s="6">
         <v>5.44815465729349E-2</v>
       </c>
       <c r="N23" s="4"/>
-      <c r="O23" s="5" t="s">
+      <c r="O23" s="24" t="s">
         <v>37</v>
       </c>
       <c r="P23" s="6">
         <v>6.2529606821411607E-2</v>
       </c>
       <c r="Q23" s="4"/>
-      <c r="R23" s="5" t="s">
+      <c r="R23" s="22" t="s">
         <v>44</v>
       </c>
       <c r="S23" s="6">
@@ -1831,51 +1815,51 @@
       <c r="U23" s="4"/>
     </row>
     <row r="24" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="14">
+      <c r="B24" s="13">
         <v>7.3718564023804903E-2</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="F24" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="G24" s="14">
+      <c r="G24" s="13">
         <v>5.4435483870967701E-2</v>
       </c>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13" t="s">
+      <c r="H24" s="12"/>
+      <c r="I24" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="J24" s="14">
+      <c r="J24" s="13">
         <v>4.7396528704939898E-2</v>
       </c>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13" t="s">
+      <c r="K24" s="12"/>
+      <c r="L24" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="M24" s="14">
+      <c r="M24" s="13">
         <v>5.1525423728813503E-2</v>
       </c>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13" t="s">
+      <c r="N24" s="12"/>
+      <c r="O24" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="P24" s="14">
+      <c r="P24" s="13">
         <v>5.9421025901472802E-2</v>
       </c>
-      <c r="Q24" s="13"/>
-      <c r="R24" s="13" t="s">
+      <c r="Q24" s="12"/>
+      <c r="R24" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="S24" s="14">
+      <c r="S24" s="13">
         <v>4.4885945548197199E-2</v>
       </c>
       <c r="T24" s="4"/>
       <c r="U24" s="4"/>
     </row>
     <row r="28" spans="1:21">
-      <c r="F28" s="27"/>
+      <c r="F28" s="25"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>